<commit_message>
update todolist, timer to gantt chart
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhpham/Desktop/milestone2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE86495-3E6F-8649-86DB-11C4CCAC51C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C201515F-8DED-2B42-80C0-61AB5553A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,6 +553,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -600,12 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1132,7 +1132,7 @@
   <dimension ref="B1:AP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1155,13 +1155,13 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="2:42" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1169,66 +1169,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="34"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="22" t="s">
+      <c r="AI2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1255,12 +1255,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1417,42 +1417,42 @@
         <v>22</v>
       </c>
       <c r="C8" s="7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D8" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
       </c>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
     </row>
     <row r="9" spans="2:42" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>

</xml_diff>